<commit_message>
commit due to error
</commit_message>
<xml_diff>
--- a/target/test-classes/test_data/hrm_data.xlsx
+++ b/target/test-classes/test_data/hrm_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLoginTest" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Username</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Balu</t>
+  </si>
+  <si>
+    <t>balu123</t>
+  </si>
+  <si>
+    <t>balu124</t>
+  </si>
+  <si>
+    <t>balu125</t>
   </si>
 </sst>
 </file>
@@ -378,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +428,39 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -429,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>